<commit_message>
Add workflow runner, update Create View node, fix download functionality and type issues
</commit_message>
<xml_diff>
--- a/model_naming.xlsx
+++ b/model_naming.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\K132177\Documents\Python Scripts\12d_pychain\12dPychain\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WebDev\Python Scripts\12dPychain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BDE7218-6A18-4D57-8837-EB13961172D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4117109F-98D2-45D1-BDB1-485CCA94DF1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{99BF9FAB-B276-4E1A-A380-3CF65DF557F2}"/>
+    <workbookView xWindow="32580" yWindow="2070" windowWidth="21600" windowHeight="12645" xr2:uid="{99BF9FAB-B276-4E1A-A380-3CF65DF557F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1320" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1314" uniqueCount="516">
   <si>
     <t>discipline</t>
   </si>
@@ -1563,6 +1563,27 @@
   </si>
   <si>
     <t>C:\Users\K132177\Documents\12d\TrainingProj\12dpychain\12dpychain</t>
+  </si>
+  <si>
+    <t>Ruthven 202 - OHW</t>
+  </si>
+  <si>
+    <t>NWP-117-C-NWA-M2D-00-MCD-ETN-DE01</t>
+  </si>
+  <si>
+    <t>NWP-117-C-NWA-M3D-00-MCD-ETN-DE01</t>
+  </si>
+  <si>
+    <t>OHW Layout</t>
+  </si>
+  <si>
+    <t>C:\pw_12d\kbr-au-pw-06\MET750\202 - Ruthven St Level Crossing\05 Civil\09 12d Model\01 Inputs Projects\OHW.12dModel</t>
+  </si>
+  <si>
+    <t>C:\pw_12d\kbr-au-pw-06\MET750\202 - Ruthven St Level Crossing\11 Train Electrical Network\04 Models</t>
+  </si>
+  <si>
+    <t>C:\pw_12d\kbr-au-pw-06\MET750\202 - Ruthven St Level Crossing\11 Train Electrical Network\04 Models\IFC</t>
   </si>
 </sst>
 </file>
@@ -1952,11 +1973,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{991550C9-844C-424D-8168-97FB11C22078}">
-  <dimension ref="A1:H251"/>
+  <dimension ref="A1:H255"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A239" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B268" sqref="B268"/>
+      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D130" sqref="D130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4788,11 +4809,12 @@
       <c r="D118" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="E118" t="s">
-        <v>2</v>
+      <c r="E118" t="str">
+        <f t="shared" ref="E118:E127" si="14">IF(ISNUMBER(SEARCH("M2D",A118)),"2D","3D")</f>
+        <v>2D</v>
       </c>
       <c r="F118" t="str">
-        <f t="shared" ref="F118:F125" si="14">RIGHT(A118, 4)</f>
+        <f t="shared" ref="F118:F125" si="15">RIGHT(A118, 4)</f>
         <v>DE61</v>
       </c>
       <c r="G118" t="s">
@@ -4815,11 +4837,12 @@
       <c r="D119" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="E119" t="s">
-        <v>2</v>
+      <c r="E119" t="str">
+        <f t="shared" si="14"/>
+        <v>2D</v>
       </c>
       <c r="F119" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>CH25</v>
       </c>
       <c r="G119" t="s">
@@ -4842,11 +4865,12 @@
       <c r="D120" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="E120" t="s">
-        <v>2</v>
+      <c r="E120" t="str">
+        <f t="shared" si="14"/>
+        <v>2D</v>
       </c>
       <c r="F120" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>DE25</v>
       </c>
       <c r="G120" t="s">
@@ -4869,11 +4893,12 @@
       <c r="D121" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="E121" t="s">
-        <v>2</v>
+      <c r="E121" t="str">
+        <f t="shared" si="14"/>
+        <v>2D</v>
       </c>
       <c r="F121" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>DE26</v>
       </c>
       <c r="G121" t="s">
@@ -4896,11 +4921,12 @@
       <c r="D122" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="E122" t="s">
-        <v>2</v>
+      <c r="E122" t="str">
+        <f t="shared" si="14"/>
+        <v>2D</v>
       </c>
       <c r="F122" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>DE60</v>
       </c>
       <c r="G122" t="s">
@@ -4923,11 +4949,12 @@
       <c r="D123" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E123" t="s">
-        <v>26</v>
+      <c r="E123" t="str">
+        <f t="shared" si="14"/>
+        <v>3D</v>
       </c>
       <c r="F123" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>EW25</v>
       </c>
       <c r="G123" t="s">
@@ -4950,11 +4977,12 @@
       <c r="D124" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E124" t="s">
-        <v>26</v>
+      <c r="E124" t="str">
+        <f t="shared" si="14"/>
+        <v>3D</v>
       </c>
       <c r="F124" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>EW26</v>
       </c>
       <c r="G124" t="s">
@@ -4977,11 +5005,12 @@
       <c r="D125" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E125" t="s">
-        <v>26</v>
+      <c r="E125" t="str">
+        <f t="shared" si="14"/>
+        <v>3D</v>
       </c>
       <c r="F125" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>TR25</v>
       </c>
       <c r="G125" t="s">
@@ -5004,11 +5033,12 @@
       <c r="D126" t="s">
         <v>461</v>
       </c>
-      <c r="E126" t="s">
-        <v>26</v>
+      <c r="E126" t="str">
+        <f t="shared" si="14"/>
+        <v>2D</v>
       </c>
       <c r="F126" t="str">
-        <f t="shared" ref="F126:F127" si="15">RIGHT(A126, 4)</f>
+        <f t="shared" ref="F126:F127" si="16">RIGHT(A126, 4)</f>
         <v>DE91</v>
       </c>
       <c r="G126" t="s">
@@ -5031,11 +5061,12 @@
       <c r="D127" s="3" t="s">
         <v>464</v>
       </c>
-      <c r="E127" t="s">
-        <v>26</v>
+      <c r="E127" t="str">
+        <f t="shared" si="14"/>
+        <v>2D</v>
       </c>
       <c r="F127" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>CR20</v>
       </c>
       <c r="G127" t="s">
@@ -5046,126 +5077,85 @@
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B128" s="2"/>
       <c r="D128" s="3"/>
-      <c r="E128" s="2"/>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="D129" s="3"/>
+        <v>509</v>
+      </c>
+      <c r="D129" s="2"/>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>303</v>
-      </c>
-      <c r="B130" t="s">
-        <v>126</v>
-      </c>
-      <c r="C130" t="s">
-        <v>106</v>
-      </c>
-      <c r="D130" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="E130" t="s">
-        <v>2</v>
+        <v>510</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C130">
+        <v>620</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="E130" t="str">
+        <f t="shared" ref="E130:E131" si="17">IF(ISNUMBER(SEARCH("M2D",A130)),"2D","3D")</f>
+        <v>2D</v>
       </c>
       <c r="F130" t="str">
-        <f t="shared" ref="F130" si="16">RIGHT(A130, 4)</f>
-        <v>DE20</v>
+        <f t="shared" ref="F130:F131" si="18">RIGHT(A130, 4)</f>
+        <v>DE01</v>
       </c>
       <c r="G130" t="s">
-        <v>217</v>
+        <v>513</v>
       </c>
       <c r="H130" t="s">
-        <v>218</v>
+        <v>514</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>297</v>
-      </c>
-      <c r="B131" t="s">
-        <v>126</v>
-      </c>
-      <c r="C131" t="s">
-        <v>106</v>
-      </c>
-      <c r="D131" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="E131" t="s">
-        <v>2</v>
+        <v>511</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C131">
+        <v>620</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="E131" t="str">
+        <f t="shared" si="17"/>
+        <v>3D</v>
       </c>
       <c r="F131" t="str">
-        <f t="shared" ref="F131:F136" si="17">RIGHT(A131, 4)</f>
-        <v>CH20</v>
+        <f t="shared" si="18"/>
+        <v>DE01</v>
       </c>
       <c r="G131" t="s">
-        <v>217</v>
+        <v>513</v>
       </c>
       <c r="H131" t="s">
-        <v>218</v>
+        <v>515</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>298</v>
-      </c>
-      <c r="B132" t="s">
-        <v>126</v>
-      </c>
-      <c r="C132" t="s">
-        <v>106</v>
-      </c>
-      <c r="D132" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="E132" t="s">
-        <v>2</v>
-      </c>
-      <c r="F132" t="str">
-        <f t="shared" si="17"/>
-        <v>CH99</v>
-      </c>
-      <c r="G132" t="s">
-        <v>217</v>
-      </c>
-      <c r="H132" t="s">
-        <v>218</v>
-      </c>
+      <c r="B132" s="2"/>
+      <c r="D132" s="4"/>
+      <c r="E132" s="2"/>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>299</v>
-      </c>
-      <c r="B133" t="s">
-        <v>126</v>
-      </c>
-      <c r="C133" t="s">
-        <v>106</v>
-      </c>
-      <c r="D133" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="E133" t="s">
-        <v>2</v>
-      </c>
-      <c r="F133" t="str">
-        <f t="shared" si="17"/>
-        <v>DE20</v>
-      </c>
-      <c r="G133" t="s">
-        <v>217</v>
-      </c>
-      <c r="H133" t="s">
-        <v>218</v>
-      </c>
+      <c r="A133" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D133" s="3"/>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="B134" t="s">
         <v>126</v>
@@ -5174,14 +5164,15 @@
         <v>106</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="E134" t="s">
-        <v>26</v>
+        <v>304</v>
+      </c>
+      <c r="E134" t="str">
+        <f t="shared" ref="E134:E140" si="19">IF(ISNUMBER(SEARCH("M2D",A134)),"2D","3D")</f>
+        <v>2D</v>
       </c>
       <c r="F134" t="str">
-        <f t="shared" si="17"/>
-        <v>DE23</v>
+        <f t="shared" ref="F134" si="20">RIGHT(A134, 4)</f>
+        <v>DE20</v>
       </c>
       <c r="G134" t="s">
         <v>217</v>
@@ -5192,7 +5183,7 @@
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B135" t="s">
         <v>126</v>
@@ -5201,14 +5192,15 @@
         <v>106</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="E135" t="s">
-        <v>26</v>
+        <v>219</v>
+      </c>
+      <c r="E135" t="str">
+        <f t="shared" si="19"/>
+        <v>2D</v>
       </c>
       <c r="F135" t="str">
-        <f t="shared" si="17"/>
-        <v>EW30</v>
+        <f t="shared" ref="F135:F140" si="21">RIGHT(A135, 4)</f>
+        <v>CH20</v>
       </c>
       <c r="G135" t="s">
         <v>217</v>
@@ -5219,7 +5211,7 @@
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B136" t="s">
         <v>126</v>
@@ -5227,15 +5219,16 @@
       <c r="C136" t="s">
         <v>106</v>
       </c>
-      <c r="D136" t="s">
-        <v>115</v>
-      </c>
-      <c r="E136" t="s">
-        <v>26</v>
+      <c r="D136" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E136" t="str">
+        <f t="shared" si="19"/>
+        <v>2D</v>
       </c>
       <c r="F136" t="str">
-        <f t="shared" si="17"/>
-        <v>TR30</v>
+        <f t="shared" si="21"/>
+        <v>CH99</v>
       </c>
       <c r="G136" t="s">
         <v>217</v>
@@ -5244,126 +5237,126 @@
         <v>218</v>
       </c>
     </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>299</v>
+      </c>
+      <c r="B137" t="s">
+        <v>126</v>
+      </c>
+      <c r="C137" t="s">
+        <v>106</v>
+      </c>
+      <c r="D137" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="E137" t="str">
+        <f t="shared" si="19"/>
+        <v>2D</v>
+      </c>
+      <c r="F137" t="str">
+        <f t="shared" si="21"/>
+        <v>DE20</v>
+      </c>
+      <c r="G137" t="s">
+        <v>217</v>
+      </c>
+      <c r="H137" t="s">
+        <v>218</v>
+      </c>
+    </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A138" s="1" t="s">
-        <v>273</v>
+      <c r="A138" t="s">
+        <v>300</v>
+      </c>
+      <c r="B138" t="s">
+        <v>126</v>
+      </c>
+      <c r="C138" t="s">
+        <v>106</v>
+      </c>
+      <c r="D138" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E138" t="str">
+        <f t="shared" si="19"/>
+        <v>3D</v>
+      </c>
+      <c r="F138" t="str">
+        <f t="shared" si="21"/>
+        <v>DE23</v>
+      </c>
+      <c r="G138" t="s">
+        <v>217</v>
+      </c>
+      <c r="H138" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>458</v>
+        <v>301</v>
       </c>
       <c r="B139" t="s">
-        <v>465</v>
+        <v>126</v>
       </c>
       <c r="C139" t="s">
-        <v>274</v>
-      </c>
-      <c r="D139" t="s">
-        <v>459</v>
+        <v>106</v>
+      </c>
+      <c r="D139" s="3" t="s">
+        <v>222</v>
       </c>
       <c r="E139" t="str">
-        <f t="shared" ref="E139:E146" si="18">IF(ISNUMBER(SEARCH("M2D",A139)),"2D","3D")</f>
+        <f t="shared" si="19"/>
         <v>3D</v>
       </c>
       <c r="F139" t="str">
-        <f t="shared" ref="F139:F146" si="19">RIGHT(A139, 4)</f>
-        <v>DE01</v>
+        <f t="shared" si="21"/>
+        <v>EW30</v>
       </c>
       <c r="G139" t="s">
-        <v>275</v>
+        <v>217</v>
       </c>
       <c r="H139" t="s">
-        <v>276</v>
+        <v>218</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>451</v>
+        <v>302</v>
       </c>
       <c r="B140" t="s">
-        <v>465</v>
+        <v>126</v>
       </c>
       <c r="C140" t="s">
-        <v>274</v>
+        <v>106</v>
       </c>
       <c r="D140" t="s">
-        <v>444</v>
+        <v>115</v>
       </c>
       <c r="E140" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>3D</v>
       </c>
       <c r="F140" t="str">
-        <f t="shared" si="19"/>
-        <v>DE21</v>
+        <f t="shared" si="21"/>
+        <v>TR30</v>
       </c>
       <c r="G140" t="s">
-        <v>275</v>
+        <v>217</v>
       </c>
       <c r="H140" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>452</v>
-      </c>
-      <c r="B141" t="s">
-        <v>465</v>
-      </c>
-      <c r="C141" t="s">
-        <v>274</v>
-      </c>
-      <c r="D141" t="s">
-        <v>445</v>
-      </c>
-      <c r="E141" t="str">
-        <f t="shared" si="18"/>
-        <v>3D</v>
-      </c>
-      <c r="F141" t="str">
-        <f t="shared" si="19"/>
-        <v>DE31</v>
-      </c>
-      <c r="G141" t="s">
-        <v>275</v>
-      </c>
-      <c r="H141" t="s">
-        <v>276</v>
+        <v>218</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>453</v>
-      </c>
-      <c r="B142" t="s">
-        <v>465</v>
-      </c>
-      <c r="C142" t="s">
-        <v>274</v>
-      </c>
-      <c r="D142" t="s">
-        <v>446</v>
-      </c>
-      <c r="E142" t="str">
-        <f t="shared" si="18"/>
-        <v>3D</v>
-      </c>
-      <c r="F142" t="str">
-        <f t="shared" si="19"/>
-        <v>DE41</v>
-      </c>
-      <c r="G142" t="s">
-        <v>275</v>
-      </c>
-      <c r="H142" t="s">
-        <v>276</v>
+      <c r="A142" s="1" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="B143" t="s">
         <v>465</v>
@@ -5372,14 +5365,14 @@
         <v>274</v>
       </c>
       <c r="D143" t="s">
-        <v>447</v>
+        <v>459</v>
       </c>
       <c r="E143" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" ref="E143:E150" si="22">IF(ISNUMBER(SEARCH("M2D",A143)),"2D","3D")</f>
         <v>3D</v>
       </c>
       <c r="F143" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" ref="F143:F150" si="23">RIGHT(A143, 4)</f>
         <v>DE01</v>
       </c>
       <c r="G143" t="s">
@@ -5391,7 +5384,7 @@
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="B144" t="s">
         <v>465</v>
@@ -5400,15 +5393,15 @@
         <v>274</v>
       </c>
       <c r="D144" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="E144" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>3D</v>
       </c>
       <c r="F144" t="str">
-        <f t="shared" si="19"/>
-        <v>DE02</v>
+        <f t="shared" si="23"/>
+        <v>DE21</v>
       </c>
       <c r="G144" t="s">
         <v>275</v>
@@ -5419,7 +5412,7 @@
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="B145" t="s">
         <v>465</v>
@@ -5428,15 +5421,15 @@
         <v>274</v>
       </c>
       <c r="D145" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="E145" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>3D</v>
       </c>
       <c r="F145" t="str">
-        <f t="shared" si="19"/>
-        <v>RW01</v>
+        <f t="shared" si="23"/>
+        <v>DE31</v>
       </c>
       <c r="G145" t="s">
         <v>275</v>
@@ -5447,7 +5440,7 @@
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="B146" t="s">
         <v>465</v>
@@ -5456,15 +5449,15 @@
         <v>274</v>
       </c>
       <c r="D146" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="E146" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>3D</v>
       </c>
       <c r="F146" t="str">
-        <f t="shared" si="19"/>
-        <v>RW11</v>
+        <f t="shared" si="23"/>
+        <v>DE41</v>
       </c>
       <c r="G146" t="s">
         <v>275</v>
@@ -5474,124 +5467,128 @@
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D147" s="2"/>
+      <c r="A147" t="s">
+        <v>455</v>
+      </c>
+      <c r="B147" t="s">
+        <v>465</v>
+      </c>
+      <c r="C147" t="s">
+        <v>274</v>
+      </c>
+      <c r="D147" t="s">
+        <v>447</v>
+      </c>
+      <c r="E147" t="str">
+        <f t="shared" si="22"/>
+        <v>3D</v>
+      </c>
+      <c r="F147" t="str">
+        <f t="shared" si="23"/>
+        <v>DE01</v>
+      </c>
+      <c r="G147" t="s">
+        <v>275</v>
+      </c>
+      <c r="H147" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>454</v>
+      </c>
+      <c r="B148" t="s">
+        <v>465</v>
+      </c>
+      <c r="C148" t="s">
+        <v>274</v>
+      </c>
+      <c r="D148" t="s">
+        <v>448</v>
+      </c>
+      <c r="E148" t="str">
+        <f t="shared" si="22"/>
+        <v>3D</v>
+      </c>
+      <c r="F148" t="str">
+        <f t="shared" si="23"/>
+        <v>DE02</v>
+      </c>
+      <c r="G148" t="s">
+        <v>275</v>
+      </c>
+      <c r="H148" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A149" s="1" t="s">
-        <v>248</v>
+      <c r="A149" t="s">
+        <v>456</v>
+      </c>
+      <c r="B149" t="s">
+        <v>465</v>
+      </c>
+      <c r="C149" t="s">
+        <v>274</v>
+      </c>
+      <c r="D149" t="s">
+        <v>449</v>
+      </c>
+      <c r="E149" t="str">
+        <f t="shared" si="22"/>
+        <v>3D</v>
+      </c>
+      <c r="F149" t="str">
+        <f t="shared" si="23"/>
+        <v>RW01</v>
+      </c>
+      <c r="G149" t="s">
+        <v>275</v>
+      </c>
+      <c r="H149" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>244</v>
+        <v>457</v>
       </c>
       <c r="B150" t="s">
-        <v>255</v>
-      </c>
-      <c r="C150" s="2" t="s">
-        <v>25</v>
+        <v>465</v>
+      </c>
+      <c r="C150" t="s">
+        <v>274</v>
       </c>
       <c r="D150" t="s">
-        <v>249</v>
-      </c>
-      <c r="E150" t="s">
-        <v>2</v>
+        <v>450</v>
+      </c>
+      <c r="E150" t="str">
+        <f t="shared" si="22"/>
+        <v>3D</v>
       </c>
       <c r="F150" t="str">
-        <f t="shared" ref="F150:F153" si="20">RIGHT(A150, 4)</f>
-        <v>CB02</v>
+        <f t="shared" si="23"/>
+        <v>RW11</v>
       </c>
       <c r="G150" t="s">
-        <v>254</v>
+        <v>275</v>
       </c>
       <c r="H150" t="s">
-        <v>253</v>
+        <v>276</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>245</v>
-      </c>
-      <c r="B151" t="s">
-        <v>255</v>
-      </c>
-      <c r="C151" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D151" t="s">
-        <v>250</v>
-      </c>
-      <c r="E151" t="s">
-        <v>2</v>
-      </c>
-      <c r="F151" t="str">
-        <f t="shared" si="20"/>
-        <v>PB01</v>
-      </c>
-      <c r="G151" t="s">
-        <v>254</v>
-      </c>
-      <c r="H151" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
-        <v>246</v>
-      </c>
-      <c r="B152" t="s">
-        <v>255</v>
-      </c>
-      <c r="C152" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D152" t="s">
-        <v>251</v>
-      </c>
-      <c r="E152" t="s">
-        <v>26</v>
-      </c>
-      <c r="F152" t="str">
-        <f t="shared" si="20"/>
-        <v>FS01</v>
-      </c>
-      <c r="G152" t="s">
-        <v>254</v>
-      </c>
-      <c r="H152" t="s">
-        <v>253</v>
-      </c>
+      <c r="D151" s="2"/>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>247</v>
-      </c>
-      <c r="B153" t="s">
-        <v>255</v>
-      </c>
-      <c r="C153" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D153" t="s">
-        <v>252</v>
-      </c>
-      <c r="E153" t="s">
-        <v>26</v>
-      </c>
-      <c r="F153" t="str">
-        <f t="shared" si="20"/>
-        <v>TR01</v>
-      </c>
-      <c r="G153" t="s">
-        <v>254</v>
-      </c>
-      <c r="H153" t="s">
-        <v>253</v>
+      <c r="A153" s="1" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>272</v>
+        <v>244</v>
       </c>
       <c r="B154" t="s">
         <v>255</v>
@@ -5600,14 +5597,14 @@
         <v>25</v>
       </c>
       <c r="D154" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="E154" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="F154" t="str">
-        <f t="shared" ref="F154" si="21">RIGHT(A154, 4)</f>
-        <v>TR02</v>
+        <f t="shared" ref="F154:F157" si="24">RIGHT(A154, 4)</f>
+        <v>CB02</v>
       </c>
       <c r="G154" t="s">
         <v>254</v>
@@ -5617,303 +5614,303 @@
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C155" s="2"/>
+      <c r="A155" t="s">
+        <v>245</v>
+      </c>
+      <c r="B155" t="s">
+        <v>255</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D155" t="s">
+        <v>250</v>
+      </c>
+      <c r="E155" t="s">
+        <v>2</v>
+      </c>
+      <c r="F155" t="str">
+        <f t="shared" si="24"/>
+        <v>PB01</v>
+      </c>
+      <c r="G155" t="s">
+        <v>254</v>
+      </c>
+      <c r="H155" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A156" s="1" t="s">
-        <v>263</v>
+      <c r="A156" t="s">
+        <v>246</v>
+      </c>
+      <c r="B156" t="s">
+        <v>255</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D156" t="s">
+        <v>251</v>
+      </c>
+      <c r="E156" t="s">
+        <v>26</v>
+      </c>
+      <c r="F156" t="str">
+        <f t="shared" si="24"/>
+        <v>FS01</v>
+      </c>
+      <c r="G156" t="s">
+        <v>254</v>
+      </c>
+      <c r="H156" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>267</v>
+        <v>247</v>
       </c>
       <c r="B157" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="C157" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D157" s="2" t="s">
-        <v>269</v>
+      <c r="D157" t="s">
+        <v>252</v>
       </c>
       <c r="E157" t="s">
         <v>26</v>
       </c>
       <c r="F157" t="str">
-        <f t="shared" ref="F157:F158" si="22">RIGHT(A157, 4)</f>
-        <v>EX01</v>
+        <f t="shared" si="24"/>
+        <v>TR01</v>
       </c>
       <c r="G157" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="H157" t="s">
-        <v>271</v>
+        <v>253</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="B158" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="C158" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D158" s="2" t="s">
-        <v>270</v>
+      <c r="D158" t="s">
+        <v>262</v>
       </c>
       <c r="E158" t="s">
         <v>26</v>
       </c>
       <c r="F158" t="str">
-        <f t="shared" si="22"/>
-        <v>EX01</v>
+        <f t="shared" ref="F158" si="25">RIGHT(A158, 4)</f>
+        <v>TR02</v>
       </c>
       <c r="G158" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="H158" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D159" s="4"/>
+      <c r="C159" s="2"/>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D160" s="3"/>
+        <v>263</v>
+      </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>175</v>
+        <v>267</v>
       </c>
       <c r="B161" t="s">
-        <v>177</v>
+        <v>264</v>
       </c>
       <c r="C161" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D161" s="4" t="s">
-        <v>178</v>
+      <c r="D161" s="2" t="s">
+        <v>269</v>
       </c>
       <c r="E161" t="s">
         <v>26</v>
       </c>
       <c r="F161" t="str">
-        <f t="shared" ref="F161:F164" si="23">RIGHT(A161, 4)</f>
+        <f t="shared" ref="F161:F162" si="26">RIGHT(A161, 4)</f>
         <v>EX01</v>
       </c>
       <c r="G161" t="s">
-        <v>180</v>
+        <v>265</v>
       </c>
       <c r="H161" t="s">
-        <v>181</v>
+        <v>271</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>176</v>
+        <v>268</v>
       </c>
       <c r="B162" t="s">
-        <v>177</v>
+        <v>264</v>
       </c>
       <c r="C162" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D162" s="4" t="s">
-        <v>179</v>
+      <c r="D162" s="2" t="s">
+        <v>270</v>
       </c>
       <c r="E162" t="s">
         <v>26</v>
       </c>
       <c r="F162" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>EX01</v>
       </c>
       <c r="G162" t="s">
+        <v>265</v>
+      </c>
+      <c r="H162" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D163" s="4"/>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A164" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D164" s="3"/>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>175</v>
+      </c>
+      <c r="B165" t="s">
+        <v>177</v>
+      </c>
+      <c r="C165" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D165" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="E165" t="s">
+        <v>26</v>
+      </c>
+      <c r="F165" t="str">
+        <f t="shared" ref="F165:F168" si="27">RIGHT(A165, 4)</f>
+        <v>EX01</v>
+      </c>
+      <c r="G165" t="s">
         <v>180</v>
       </c>
-      <c r="H162" t="s">
+      <c r="H165" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>176</v>
+      </c>
+      <c r="B166" t="s">
+        <v>177</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D166" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="E166" t="s">
+        <v>26</v>
+      </c>
+      <c r="F166" t="str">
+        <f t="shared" si="27"/>
+        <v>EX01</v>
+      </c>
+      <c r="G166" t="s">
+        <v>180</v>
+      </c>
+      <c r="H166" t="s">
         <v>296</v>
-      </c>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
-        <v>291</v>
-      </c>
-      <c r="B163" t="s">
-        <v>177</v>
-      </c>
-      <c r="C163" t="s">
-        <v>293</v>
-      </c>
-      <c r="D163" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="E163" t="s">
-        <v>26</v>
-      </c>
-      <c r="F163" t="str">
-        <f t="shared" si="23"/>
-        <v>AB01</v>
-      </c>
-      <c r="G163" t="s">
-        <v>180</v>
-      </c>
-      <c r="H163" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
-        <v>292</v>
-      </c>
-      <c r="B164" t="s">
-        <v>177</v>
-      </c>
-      <c r="C164" t="s">
-        <v>293</v>
-      </c>
-      <c r="D164" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="E164" t="s">
-        <v>26</v>
-      </c>
-      <c r="F164" t="str">
-        <f t="shared" si="23"/>
-        <v>AB01</v>
-      </c>
-      <c r="G164" t="s">
-        <v>180</v>
-      </c>
-      <c r="H164" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D165" s="3"/>
-    </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A166" s="1" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="B167" t="s">
-        <v>126</v>
+        <v>177</v>
       </c>
       <c r="C167" t="s">
-        <v>106</v>
-      </c>
-      <c r="D167" t="s">
-        <v>306</v>
+        <v>293</v>
+      </c>
+      <c r="D167" s="3" t="s">
+        <v>294</v>
       </c>
       <c r="E167" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="F167" t="str">
-        <f t="shared" ref="F167:F187" si="24">RIGHT(A167, 4)</f>
-        <v>CH01</v>
+        <f t="shared" si="27"/>
+        <v>AB01</v>
       </c>
       <c r="G167" t="s">
-        <v>348</v>
+        <v>180</v>
       </c>
       <c r="H167" t="s">
-        <v>307</v>
+        <v>182</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
       <c r="B168" t="s">
-        <v>126</v>
+        <v>177</v>
       </c>
       <c r="C168" t="s">
-        <v>106</v>
-      </c>
-      <c r="D168" t="s">
-        <v>309</v>
+        <v>293</v>
+      </c>
+      <c r="D168" s="3" t="s">
+        <v>295</v>
       </c>
       <c r="E168" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="F168" t="str">
-        <f t="shared" si="24"/>
-        <v>CH10</v>
+        <f t="shared" si="27"/>
+        <v>AB01</v>
       </c>
       <c r="G168" t="s">
-        <v>348</v>
+        <v>180</v>
       </c>
       <c r="H168" t="s">
-        <v>307</v>
+        <v>181</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
-        <v>310</v>
-      </c>
-      <c r="B169" t="s">
-        <v>126</v>
-      </c>
-      <c r="C169" t="s">
-        <v>106</v>
-      </c>
-      <c r="D169" t="s">
-        <v>311</v>
-      </c>
-      <c r="E169" t="s">
-        <v>2</v>
-      </c>
-      <c r="F169" t="str">
-        <f t="shared" si="24"/>
-        <v>CH30</v>
-      </c>
-      <c r="G169" t="s">
-        <v>348</v>
-      </c>
-      <c r="H169" t="s">
-        <v>307</v>
-      </c>
+      <c r="D169" s="3"/>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
-        <v>312</v>
-      </c>
-      <c r="B170" t="s">
-        <v>126</v>
-      </c>
-      <c r="C170" t="s">
-        <v>106</v>
-      </c>
-      <c r="D170" t="s">
-        <v>313</v>
-      </c>
-      <c r="E170" t="s">
-        <v>2</v>
-      </c>
-      <c r="F170" t="str">
-        <f t="shared" si="24"/>
-        <v>CH80</v>
-      </c>
-      <c r="G170" t="s">
-        <v>348</v>
-      </c>
-      <c r="H170" t="s">
-        <v>307</v>
+      <c r="A170" s="1" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="B171" t="s">
         <v>126</v>
@@ -5922,14 +5919,14 @@
         <v>106</v>
       </c>
       <c r="D171" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E171" t="s">
         <v>2</v>
       </c>
       <c r="F171" t="str">
-        <f t="shared" si="24"/>
-        <v>CH90</v>
+        <f t="shared" ref="F171:F191" si="28">RIGHT(A171, 4)</f>
+        <v>CH01</v>
       </c>
       <c r="G171" t="s">
         <v>348</v>
@@ -5940,7 +5937,7 @@
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="B172" t="s">
         <v>126</v>
@@ -5949,14 +5946,14 @@
         <v>106</v>
       </c>
       <c r="D172" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="E172" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="F172" t="str">
-        <f t="shared" si="24"/>
-        <v>DE01</v>
+        <f t="shared" si="28"/>
+        <v>CH10</v>
       </c>
       <c r="G172" t="s">
         <v>348</v>
@@ -5967,7 +5964,7 @@
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B173" t="s">
         <v>126</v>
@@ -5976,14 +5973,14 @@
         <v>106</v>
       </c>
       <c r="D173" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="E173" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="F173" t="str">
-        <f t="shared" si="24"/>
-        <v>DE80</v>
+        <f t="shared" si="28"/>
+        <v>CH30</v>
       </c>
       <c r="G173" t="s">
         <v>348</v>
@@ -5994,7 +5991,7 @@
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="B174" t="s">
         <v>126</v>
@@ -6003,14 +6000,14 @@
         <v>106</v>
       </c>
       <c r="D174" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="E174" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="F174" t="str">
-        <f t="shared" si="24"/>
-        <v>DE90</v>
+        <f t="shared" si="28"/>
+        <v>CH80</v>
       </c>
       <c r="G174" t="s">
         <v>348</v>
@@ -6021,7 +6018,7 @@
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="B175" t="s">
         <v>126</v>
@@ -6030,14 +6027,14 @@
         <v>106</v>
       </c>
       <c r="D175" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="E175" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="F175" t="str">
-        <f t="shared" si="24"/>
-        <v>EW10</v>
+        <f t="shared" si="28"/>
+        <v>CH90</v>
       </c>
       <c r="G175" t="s">
         <v>348</v>
@@ -6048,7 +6045,7 @@
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="B176" t="s">
         <v>126</v>
@@ -6057,14 +6054,14 @@
         <v>106</v>
       </c>
       <c r="D176" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="E176" t="s">
         <v>26</v>
       </c>
       <c r="F176" t="str">
-        <f t="shared" si="24"/>
-        <v>EW80</v>
+        <f t="shared" si="28"/>
+        <v>DE01</v>
       </c>
       <c r="G176" t="s">
         <v>348</v>
@@ -6075,7 +6072,7 @@
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="B177" t="s">
         <v>126</v>
@@ -6084,14 +6081,14 @@
         <v>106</v>
       </c>
       <c r="D177" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="E177" t="s">
         <v>26</v>
       </c>
       <c r="F177" t="str">
-        <f t="shared" si="24"/>
-        <v>EW90</v>
+        <f t="shared" si="28"/>
+        <v>DE80</v>
       </c>
       <c r="G177" t="s">
         <v>348</v>
@@ -6102,7 +6099,7 @@
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="B178" t="s">
         <v>126</v>
@@ -6111,14 +6108,14 @@
         <v>106</v>
       </c>
       <c r="D178" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="E178" t="s">
         <v>26</v>
       </c>
       <c r="F178" t="str">
-        <f t="shared" si="24"/>
-        <v>TR10</v>
+        <f t="shared" si="28"/>
+        <v>DE90</v>
       </c>
       <c r="G178" t="s">
         <v>348</v>
@@ -6129,7 +6126,7 @@
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="B179" t="s">
         <v>126</v>
@@ -6138,14 +6135,14 @@
         <v>106</v>
       </c>
       <c r="D179" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="E179" t="s">
         <v>26</v>
       </c>
       <c r="F179" t="str">
-        <f t="shared" si="24"/>
-        <v>TR20</v>
+        <f t="shared" si="28"/>
+        <v>EW10</v>
       </c>
       <c r="G179" t="s">
         <v>348</v>
@@ -6156,7 +6153,7 @@
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="B180" t="s">
         <v>126</v>
@@ -6165,14 +6162,14 @@
         <v>106</v>
       </c>
       <c r="D180" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="E180" t="s">
         <v>26</v>
       </c>
       <c r="F180" t="str">
-        <f t="shared" si="24"/>
-        <v>TR30</v>
+        <f t="shared" si="28"/>
+        <v>EW80</v>
       </c>
       <c r="G180" t="s">
         <v>348</v>
@@ -6183,7 +6180,7 @@
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="B181" t="s">
         <v>126</v>
@@ -6192,14 +6189,14 @@
         <v>106</v>
       </c>
       <c r="D181" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="E181" t="s">
         <v>26</v>
       </c>
       <c r="F181" t="str">
-        <f t="shared" si="24"/>
-        <v>TR40</v>
+        <f t="shared" si="28"/>
+        <v>EW90</v>
       </c>
       <c r="G181" t="s">
         <v>348</v>
@@ -6210,7 +6207,7 @@
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="B182" t="s">
         <v>126</v>
@@ -6219,14 +6216,14 @@
         <v>106</v>
       </c>
       <c r="D182" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="E182" t="s">
         <v>26</v>
       </c>
       <c r="F182" t="str">
-        <f t="shared" si="24"/>
-        <v>TR60</v>
+        <f t="shared" si="28"/>
+        <v>TR10</v>
       </c>
       <c r="G182" t="s">
         <v>348</v>
@@ -6237,7 +6234,7 @@
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="B183" t="s">
         <v>126</v>
@@ -6246,14 +6243,14 @@
         <v>106</v>
       </c>
       <c r="D183" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="E183" t="s">
         <v>26</v>
       </c>
       <c r="F183" t="str">
-        <f t="shared" si="24"/>
-        <v>TR70</v>
+        <f t="shared" si="28"/>
+        <v>TR20</v>
       </c>
       <c r="G183" t="s">
         <v>348</v>
@@ -6264,7 +6261,7 @@
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="B184" t="s">
         <v>126</v>
@@ -6273,14 +6270,14 @@
         <v>106</v>
       </c>
       <c r="D184" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="E184" t="s">
         <v>26</v>
       </c>
       <c r="F184" t="str">
-        <f t="shared" si="24"/>
-        <v>TR80</v>
+        <f t="shared" si="28"/>
+        <v>TR30</v>
       </c>
       <c r="G184" t="s">
         <v>348</v>
@@ -6291,7 +6288,7 @@
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="B185" t="s">
         <v>126</v>
@@ -6300,14 +6297,14 @@
         <v>106</v>
       </c>
       <c r="D185" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="E185" t="s">
         <v>26</v>
       </c>
       <c r="F185" t="str">
-        <f t="shared" si="24"/>
-        <v>TR90</v>
+        <f t="shared" si="28"/>
+        <v>TR40</v>
       </c>
       <c r="G185" t="s">
         <v>348</v>
@@ -6318,7 +6315,7 @@
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="B186" t="s">
         <v>126</v>
@@ -6327,14 +6324,14 @@
         <v>106</v>
       </c>
       <c r="D186" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="E186" t="s">
         <v>26</v>
       </c>
       <c r="F186" t="str">
-        <f t="shared" si="24"/>
-        <v>DE70</v>
+        <f t="shared" si="28"/>
+        <v>TR60</v>
       </c>
       <c r="G186" t="s">
         <v>348</v>
@@ -6345,7 +6342,7 @@
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="B187" t="s">
         <v>126</v>
@@ -6354,14 +6351,14 @@
         <v>106</v>
       </c>
       <c r="D187" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="E187" t="s">
         <v>26</v>
       </c>
       <c r="F187" t="str">
-        <f t="shared" si="24"/>
-        <v>DE90</v>
+        <f t="shared" si="28"/>
+        <v>TR70</v>
       </c>
       <c r="G187" t="s">
         <v>348</v>
@@ -6370,126 +6367,122 @@
         <v>307</v>
       </c>
     </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>340</v>
+      </c>
+      <c r="B188" t="s">
+        <v>126</v>
+      </c>
+      <c r="C188" t="s">
+        <v>106</v>
+      </c>
+      <c r="D188" t="s">
+        <v>341</v>
+      </c>
+      <c r="E188" t="s">
+        <v>26</v>
+      </c>
+      <c r="F188" t="str">
+        <f t="shared" si="28"/>
+        <v>TR80</v>
+      </c>
+      <c r="G188" t="s">
+        <v>348</v>
+      </c>
+      <c r="H188" t="s">
+        <v>307</v>
+      </c>
+    </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A189" s="1" t="s">
-        <v>387</v>
+      <c r="A189" t="s">
+        <v>342</v>
+      </c>
+      <c r="B189" t="s">
+        <v>126</v>
+      </c>
+      <c r="C189" t="s">
+        <v>106</v>
+      </c>
+      <c r="D189" t="s">
+        <v>343</v>
+      </c>
+      <c r="E189" t="s">
+        <v>26</v>
+      </c>
+      <c r="F189" t="str">
+        <f t="shared" si="28"/>
+        <v>TR90</v>
+      </c>
+      <c r="G189" t="s">
+        <v>348</v>
+      </c>
+      <c r="H189" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="B190" t="s">
-        <v>366</v>
+        <v>126</v>
       </c>
       <c r="C190" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="D190" t="s">
-        <v>369</v>
-      </c>
-      <c r="E190" t="str">
-        <f>IF(ISNUMBER(SEARCH("M2D",A190)),"2D","3D")</f>
-        <v>3D</v>
+        <v>345</v>
+      </c>
+      <c r="E190" t="s">
+        <v>26</v>
       </c>
       <c r="F190" t="str">
-        <f t="shared" ref="F190:F206" si="25">RIGHT(A190, 4)</f>
-        <v>TR30</v>
+        <f t="shared" si="28"/>
+        <v>DE70</v>
       </c>
       <c r="G190" t="s">
-        <v>389</v>
+        <v>348</v>
       </c>
       <c r="H190" t="s">
-        <v>388</v>
+        <v>307</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="B191" t="s">
-        <v>367</v>
+        <v>126</v>
       </c>
       <c r="C191" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="D191" t="s">
-        <v>370</v>
-      </c>
-      <c r="E191" t="str">
-        <f t="shared" ref="E191:E206" si="26">IF(ISNUMBER(SEARCH("M2D",A191)),"2D","3D")</f>
-        <v>3D</v>
+        <v>347</v>
+      </c>
+      <c r="E191" t="s">
+        <v>26</v>
       </c>
       <c r="F191" t="str">
-        <f t="shared" si="25"/>
-        <v>TR02</v>
+        <f t="shared" si="28"/>
+        <v>DE90</v>
       </c>
       <c r="G191" t="s">
-        <v>389</v>
+        <v>348</v>
       </c>
       <c r="H191" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
-        <v>351</v>
-      </c>
-      <c r="B192" t="s">
-        <v>367</v>
-      </c>
-      <c r="C192" t="s">
-        <v>122</v>
-      </c>
-      <c r="D192" t="s">
-        <v>371</v>
-      </c>
-      <c r="E192" t="str">
-        <f t="shared" si="26"/>
-        <v>3D</v>
-      </c>
-      <c r="F192" t="str">
-        <f t="shared" si="25"/>
-        <v>TR34</v>
-      </c>
-      <c r="G192" t="s">
-        <v>389</v>
-      </c>
-      <c r="H192" t="s">
-        <v>388</v>
+        <v>307</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A193" t="s">
-        <v>352</v>
-      </c>
-      <c r="B193" t="s">
-        <v>367</v>
-      </c>
-      <c r="C193" t="s">
-        <v>122</v>
-      </c>
-      <c r="D193" t="s">
-        <v>372</v>
-      </c>
-      <c r="E193" t="str">
-        <f t="shared" si="26"/>
-        <v>3D</v>
-      </c>
-      <c r="F193" t="str">
-        <f t="shared" si="25"/>
-        <v>TR38</v>
-      </c>
-      <c r="G193" t="s">
-        <v>389</v>
-      </c>
-      <c r="H193" t="s">
-        <v>388</v>
+      <c r="A193" s="1" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="B194" t="s">
         <v>366</v>
@@ -6498,15 +6491,15 @@
         <v>122</v>
       </c>
       <c r="D194" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E194" t="str">
-        <f t="shared" si="26"/>
+        <f>IF(ISNUMBER(SEARCH("M2D",A194)),"2D","3D")</f>
         <v>3D</v>
       </c>
       <c r="F194" t="str">
-        <f t="shared" si="25"/>
-        <v>TR31</v>
+        <f t="shared" ref="F194:F210" si="29">RIGHT(A194, 4)</f>
+        <v>TR30</v>
       </c>
       <c r="G194" t="s">
         <v>389</v>
@@ -6517,7 +6510,7 @@
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="B195" t="s">
         <v>367</v>
@@ -6526,15 +6519,15 @@
         <v>122</v>
       </c>
       <c r="D195" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="E195" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" ref="E195:E210" si="30">IF(ISNUMBER(SEARCH("M2D",A195)),"2D","3D")</f>
         <v>3D</v>
       </c>
       <c r="F195" t="str">
-        <f t="shared" si="25"/>
-        <v>TR20</v>
+        <f t="shared" si="29"/>
+        <v>TR02</v>
       </c>
       <c r="G195" t="s">
         <v>389</v>
@@ -6545,24 +6538,24 @@
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B196" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C196" t="s">
         <v>122</v>
       </c>
       <c r="D196" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="E196" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>3D</v>
       </c>
       <c r="F196" t="str">
-        <f t="shared" si="25"/>
-        <v>TR41</v>
+        <f t="shared" si="29"/>
+        <v>TR34</v>
       </c>
       <c r="G196" t="s">
         <v>389</v>
@@ -6573,24 +6566,24 @@
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="B197" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C197" t="s">
         <v>122</v>
       </c>
       <c r="D197" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="E197" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>3D</v>
       </c>
       <c r="F197" t="str">
-        <f t="shared" si="25"/>
-        <v>TR21</v>
+        <f t="shared" si="29"/>
+        <v>TR38</v>
       </c>
       <c r="G197" t="s">
         <v>389</v>
@@ -6601,24 +6594,24 @@
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="B198" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C198" t="s">
         <v>122</v>
       </c>
       <c r="D198" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="E198" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>3D</v>
       </c>
       <c r="F198" t="str">
-        <f t="shared" si="25"/>
-        <v>TR33</v>
+        <f t="shared" si="29"/>
+        <v>TR31</v>
       </c>
       <c r="G198" t="s">
         <v>389</v>
@@ -6629,24 +6622,24 @@
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B199" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C199" t="s">
         <v>122</v>
       </c>
       <c r="D199" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="E199" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>3D</v>
       </c>
       <c r="F199" t="str">
-        <f t="shared" si="25"/>
-        <v>EW30</v>
+        <f t="shared" si="29"/>
+        <v>TR20</v>
       </c>
       <c r="G199" t="s">
         <v>389</v>
@@ -6657,24 +6650,24 @@
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B200" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C200" t="s">
         <v>122</v>
       </c>
       <c r="D200" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="E200" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>3D</v>
       </c>
       <c r="F200" t="str">
-        <f t="shared" si="25"/>
-        <v>EW34</v>
+        <f t="shared" si="29"/>
+        <v>TR41</v>
       </c>
       <c r="G200" t="s">
         <v>389</v>
@@ -6685,24 +6678,24 @@
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B201" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C201" t="s">
         <v>122</v>
       </c>
       <c r="D201" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="E201" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>3D</v>
       </c>
       <c r="F201" t="str">
-        <f t="shared" si="25"/>
-        <v>EW38</v>
+        <f t="shared" si="29"/>
+        <v>TR21</v>
       </c>
       <c r="G201" t="s">
         <v>389</v>
@@ -6713,24 +6706,24 @@
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B202" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="C202" t="s">
         <v>122</v>
       </c>
       <c r="D202" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="E202" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>3D</v>
       </c>
       <c r="F202" t="str">
-        <f t="shared" si="25"/>
-        <v>EW31</v>
+        <f t="shared" si="29"/>
+        <v>TR33</v>
       </c>
       <c r="G202" t="s">
         <v>389</v>
@@ -6741,24 +6734,24 @@
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="B203" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C203" t="s">
         <v>122</v>
       </c>
       <c r="D203" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="E203" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>3D</v>
       </c>
       <c r="F203" t="str">
-        <f t="shared" si="25"/>
-        <v>EW20</v>
+        <f t="shared" si="29"/>
+        <v>EW30</v>
       </c>
       <c r="G203" t="s">
         <v>389</v>
@@ -6769,24 +6762,24 @@
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B204" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C204" t="s">
         <v>122</v>
       </c>
       <c r="D204" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="E204" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>3D</v>
       </c>
       <c r="F204" t="str">
-        <f t="shared" si="25"/>
-        <v>EW41</v>
+        <f t="shared" si="29"/>
+        <v>EW34</v>
       </c>
       <c r="G204" t="s">
         <v>389</v>
@@ -6797,24 +6790,24 @@
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="B205" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C205" t="s">
         <v>122</v>
       </c>
       <c r="D205" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="E205" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>3D</v>
       </c>
       <c r="F205" t="str">
-        <f t="shared" si="25"/>
-        <v>EW33</v>
+        <f t="shared" si="29"/>
+        <v>EW38</v>
       </c>
       <c r="G205" t="s">
         <v>389</v>
@@ -6825,24 +6818,24 @@
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="B206" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C206" t="s">
         <v>122</v>
       </c>
       <c r="D206" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="E206" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>3D</v>
       </c>
       <c r="F206" t="str">
-        <f t="shared" si="25"/>
-        <v>EW21</v>
+        <f t="shared" si="29"/>
+        <v>EW31</v>
       </c>
       <c r="G206" t="s">
         <v>389</v>
@@ -6851,126 +6844,126 @@
         <v>388</v>
       </c>
     </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>362</v>
+      </c>
+      <c r="B207" t="s">
+        <v>367</v>
+      </c>
+      <c r="C207" t="s">
+        <v>122</v>
+      </c>
+      <c r="D207" t="s">
+        <v>382</v>
+      </c>
+      <c r="E207" t="str">
+        <f t="shared" si="30"/>
+        <v>3D</v>
+      </c>
+      <c r="F207" t="str">
+        <f t="shared" si="29"/>
+        <v>EW20</v>
+      </c>
+      <c r="G207" t="s">
+        <v>389</v>
+      </c>
+      <c r="H207" t="s">
+        <v>388</v>
+      </c>
+    </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A208" s="1" t="s">
-        <v>390</v>
+      <c r="A208" t="s">
+        <v>363</v>
+      </c>
+      <c r="B208" t="s">
+        <v>366</v>
+      </c>
+      <c r="C208" t="s">
+        <v>122</v>
+      </c>
+      <c r="D208" t="s">
+        <v>383</v>
+      </c>
+      <c r="E208" t="str">
+        <f t="shared" si="30"/>
+        <v>3D</v>
+      </c>
+      <c r="F208" t="str">
+        <f t="shared" si="29"/>
+        <v>EW41</v>
+      </c>
+      <c r="G208" t="s">
+        <v>389</v>
+      </c>
+      <c r="H208" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>391</v>
+        <v>364</v>
       </c>
       <c r="B209" t="s">
-        <v>402</v>
+        <v>368</v>
       </c>
       <c r="C209" t="s">
-        <v>274</v>
+        <v>122</v>
       </c>
       <c r="D209" t="s">
-        <v>405</v>
+        <v>384</v>
       </c>
       <c r="E209" t="str">
-        <f t="shared" ref="E209:E234" si="27">IF(ISNUMBER(SEARCH("M2D",A209)),"2D","3D")</f>
+        <f t="shared" si="30"/>
         <v>3D</v>
       </c>
       <c r="F209" t="str">
-        <f t="shared" ref="F209:F234" si="28">RIGHT(A209, 4)</f>
-        <v>DE01</v>
+        <f t="shared" si="29"/>
+        <v>EW33</v>
       </c>
       <c r="G209" t="s">
-        <v>443</v>
+        <v>389</v>
       </c>
       <c r="H209" t="s">
-        <v>442</v>
+        <v>388</v>
       </c>
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>392</v>
+        <v>365</v>
       </c>
       <c r="B210" t="s">
-        <v>402</v>
+        <v>368</v>
       </c>
       <c r="C210" t="s">
-        <v>274</v>
+        <v>122</v>
       </c>
       <c r="D210" t="s">
-        <v>406</v>
+        <v>385</v>
       </c>
       <c r="E210" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>3D</v>
       </c>
       <c r="F210" t="str">
-        <f t="shared" si="28"/>
-        <v>DE11</v>
+        <f t="shared" si="29"/>
+        <v>EW21</v>
       </c>
       <c r="G210" t="s">
-        <v>443</v>
+        <v>389</v>
       </c>
       <c r="H210" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A211" t="s">
-        <v>394</v>
-      </c>
-      <c r="B211" t="s">
-        <v>402</v>
-      </c>
-      <c r="C211" t="s">
-        <v>274</v>
-      </c>
-      <c r="D211" t="s">
-        <v>407</v>
-      </c>
-      <c r="E211" t="str">
-        <f t="shared" si="27"/>
-        <v>3D</v>
-      </c>
-      <c r="F211" t="str">
-        <f t="shared" si="28"/>
-        <v>DE21</v>
-      </c>
-      <c r="G211" t="s">
-        <v>443</v>
-      </c>
-      <c r="H211" t="s">
-        <v>442</v>
+        <v>388</v>
       </c>
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A212" t="s">
-        <v>393</v>
-      </c>
-      <c r="B212" t="s">
-        <v>402</v>
-      </c>
-      <c r="C212" t="s">
-        <v>274</v>
-      </c>
-      <c r="D212" t="s">
-        <v>408</v>
-      </c>
-      <c r="E212" t="str">
-        <f t="shared" si="27"/>
-        <v>3D</v>
-      </c>
-      <c r="F212" t="str">
-        <f t="shared" si="28"/>
-        <v>DE26</v>
-      </c>
-      <c r="G212" t="s">
-        <v>443</v>
-      </c>
-      <c r="H212" t="s">
-        <v>442</v>
+      <c r="A212" s="1" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B213" t="s">
         <v>402</v>
@@ -6979,14 +6972,14 @@
         <v>274</v>
       </c>
       <c r="D213" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="E213" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" ref="E213:E238" si="31">IF(ISNUMBER(SEARCH("M2D",A213)),"2D","3D")</f>
         <v>3D</v>
       </c>
       <c r="F213" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" ref="F213:F238" si="32">RIGHT(A213, 4)</f>
         <v>DE01</v>
       </c>
       <c r="G213" t="s">
@@ -6998,7 +6991,7 @@
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="B214" t="s">
         <v>402</v>
@@ -7007,15 +7000,15 @@
         <v>274</v>
       </c>
       <c r="D214" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="E214" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3D</v>
       </c>
       <c r="F214" t="str">
-        <f t="shared" si="28"/>
-        <v>RW01</v>
+        <f t="shared" si="32"/>
+        <v>DE11</v>
       </c>
       <c r="G214" t="s">
         <v>443</v>
@@ -7026,7 +7019,7 @@
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="B215" t="s">
         <v>402</v>
@@ -7035,15 +7028,15 @@
         <v>274</v>
       </c>
       <c r="D215" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="E215" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3D</v>
       </c>
       <c r="F215" t="str">
-        <f t="shared" si="28"/>
-        <v>RW11</v>
+        <f t="shared" si="32"/>
+        <v>DE21</v>
       </c>
       <c r="G215" t="s">
         <v>443</v>
@@ -7054,24 +7047,24 @@
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="B216" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C216" t="s">
         <v>274</v>
       </c>
       <c r="D216" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="E216" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3D</v>
       </c>
       <c r="F216" t="str">
-        <f t="shared" si="28"/>
-        <v>DE01</v>
+        <f t="shared" si="32"/>
+        <v>DE26</v>
       </c>
       <c r="G216" t="s">
         <v>443</v>
@@ -7082,24 +7075,24 @@
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="B217" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C217" t="s">
         <v>274</v>
       </c>
       <c r="D217" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="E217" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3D</v>
       </c>
       <c r="F217" t="str">
-        <f t="shared" si="28"/>
-        <v>DE02</v>
+        <f t="shared" si="32"/>
+        <v>DE01</v>
       </c>
       <c r="G217" t="s">
         <v>443</v>
@@ -7110,24 +7103,24 @@
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="B218" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C218" t="s">
         <v>274</v>
       </c>
       <c r="D218" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="E218" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3D</v>
       </c>
       <c r="F218" t="str">
-        <f t="shared" si="28"/>
-        <v>DE41</v>
+        <f t="shared" si="32"/>
+        <v>RW01</v>
       </c>
       <c r="G218" t="s">
         <v>443</v>
@@ -7138,24 +7131,24 @@
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="B219" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C219" t="s">
         <v>274</v>
       </c>
       <c r="D219" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="E219" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3D</v>
       </c>
       <c r="F219" t="str">
-        <f t="shared" si="28"/>
-        <v>DE01</v>
+        <f t="shared" si="32"/>
+        <v>RW11</v>
       </c>
       <c r="G219" t="s">
         <v>443</v>
@@ -7166,7 +7159,7 @@
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>427</v>
+        <v>398</v>
       </c>
       <c r="B220" t="s">
         <v>403</v>
@@ -7175,15 +7168,15 @@
         <v>274</v>
       </c>
       <c r="D220" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="E220" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3D</v>
       </c>
       <c r="F220" t="str">
-        <f t="shared" si="28"/>
-        <v>RW33</v>
+        <f t="shared" si="32"/>
+        <v>DE01</v>
       </c>
       <c r="G220" t="s">
         <v>443</v>
@@ -7194,24 +7187,24 @@
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>428</v>
+        <v>400</v>
       </c>
       <c r="B221" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C221" t="s">
         <v>274</v>
       </c>
       <c r="D221" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="E221" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3D</v>
       </c>
       <c r="F221" t="str">
-        <f t="shared" si="28"/>
-        <v>DE01</v>
+        <f t="shared" si="32"/>
+        <v>DE02</v>
       </c>
       <c r="G221" t="s">
         <v>443</v>
@@ -7222,24 +7215,24 @@
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>429</v>
+        <v>399</v>
       </c>
       <c r="B222" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C222" t="s">
         <v>274</v>
       </c>
       <c r="D222" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="E222" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3D</v>
       </c>
       <c r="F222" t="str">
-        <f t="shared" si="28"/>
-        <v>DE11</v>
+        <f t="shared" si="32"/>
+        <v>DE41</v>
       </c>
       <c r="G222" t="s">
         <v>443</v>
@@ -7250,24 +7243,24 @@
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>430</v>
+        <v>401</v>
       </c>
       <c r="B223" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C223" t="s">
         <v>274</v>
       </c>
       <c r="D223" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
       <c r="E223" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3D</v>
       </c>
       <c r="F223" t="str">
-        <f t="shared" si="28"/>
-        <v>DE21</v>
+        <f t="shared" si="32"/>
+        <v>DE01</v>
       </c>
       <c r="G223" t="s">
         <v>443</v>
@@ -7278,24 +7271,24 @@
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="B224" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C224" t="s">
         <v>274</v>
       </c>
       <c r="D224" t="s">
-        <v>408</v>
+        <v>415</v>
       </c>
       <c r="E224" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3D</v>
       </c>
       <c r="F224" t="str">
-        <f t="shared" si="28"/>
-        <v>DE26</v>
+        <f t="shared" si="32"/>
+        <v>RW33</v>
       </c>
       <c r="G224" t="s">
         <v>443</v>
@@ -7306,7 +7299,7 @@
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="B225" t="s">
         <v>404</v>
@@ -7315,15 +7308,15 @@
         <v>274</v>
       </c>
       <c r="D225" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="E225" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3D</v>
       </c>
       <c r="F225" t="str">
-        <f t="shared" si="28"/>
-        <v>DE31</v>
+        <f t="shared" si="32"/>
+        <v>DE01</v>
       </c>
       <c r="G225" t="s">
         <v>443</v>
@@ -7334,7 +7327,7 @@
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="B226" t="s">
         <v>404</v>
@@ -7343,15 +7336,15 @@
         <v>274</v>
       </c>
       <c r="D226" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="E226" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3D</v>
       </c>
       <c r="F226" t="str">
-        <f t="shared" si="28"/>
-        <v>DE32</v>
+        <f t="shared" si="32"/>
+        <v>DE11</v>
       </c>
       <c r="G226" t="s">
         <v>443</v>
@@ -7362,7 +7355,7 @@
     </row>
     <row r="227" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="B227" t="s">
         <v>404</v>
@@ -7371,15 +7364,15 @@
         <v>274</v>
       </c>
       <c r="D227" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="E227" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3D</v>
       </c>
       <c r="F227" t="str">
-        <f t="shared" si="28"/>
-        <v>DE36</v>
+        <f t="shared" si="32"/>
+        <v>DE21</v>
       </c>
       <c r="G227" t="s">
         <v>443</v>
@@ -7390,7 +7383,7 @@
     </row>
     <row r="228" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="B228" t="s">
         <v>404</v>
@@ -7399,15 +7392,15 @@
         <v>274</v>
       </c>
       <c r="D228" t="s">
-        <v>422</v>
+        <v>408</v>
       </c>
       <c r="E228" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3D</v>
       </c>
       <c r="F228" t="str">
-        <f t="shared" si="28"/>
-        <v>DE37</v>
+        <f t="shared" si="32"/>
+        <v>DE26</v>
       </c>
       <c r="G228" t="s">
         <v>443</v>
@@ -7418,7 +7411,7 @@
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="B229" t="s">
         <v>404</v>
@@ -7427,15 +7420,15 @@
         <v>274</v>
       </c>
       <c r="D229" t="s">
-        <v>409</v>
+        <v>419</v>
       </c>
       <c r="E229" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3D</v>
       </c>
       <c r="F229" t="str">
-        <f t="shared" si="28"/>
-        <v>DE01</v>
+        <f t="shared" si="32"/>
+        <v>DE31</v>
       </c>
       <c r="G229" t="s">
         <v>443</v>
@@ -7446,7 +7439,7 @@
     </row>
     <row r="230" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="B230" t="s">
         <v>404</v>
@@ -7455,15 +7448,15 @@
         <v>274</v>
       </c>
       <c r="D230" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="E230" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3D</v>
       </c>
       <c r="F230" t="str">
-        <f t="shared" si="28"/>
-        <v>RW21</v>
+        <f t="shared" si="32"/>
+        <v>DE32</v>
       </c>
       <c r="G230" t="s">
         <v>443</v>
@@ -7474,7 +7467,7 @@
     </row>
     <row r="231" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="B231" t="s">
         <v>404</v>
@@ -7483,15 +7476,15 @@
         <v>274</v>
       </c>
       <c r="D231" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="E231" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3D</v>
       </c>
       <c r="F231" t="str">
-        <f t="shared" si="28"/>
-        <v>RW31</v>
+        <f t="shared" si="32"/>
+        <v>DE36</v>
       </c>
       <c r="G231" t="s">
         <v>443</v>
@@ -7502,7 +7495,7 @@
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="B232" t="s">
         <v>404</v>
@@ -7511,15 +7504,15 @@
         <v>274</v>
       </c>
       <c r="D232" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="E232" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3D</v>
       </c>
       <c r="F232" t="str">
-        <f t="shared" si="28"/>
-        <v>RW32</v>
+        <f t="shared" si="32"/>
+        <v>DE37</v>
       </c>
       <c r="G232" t="s">
         <v>443</v>
@@ -7530,7 +7523,7 @@
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="B233" t="s">
         <v>404</v>
@@ -7539,15 +7532,15 @@
         <v>274</v>
       </c>
       <c r="D233" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="E233" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3D</v>
       </c>
       <c r="F233" t="str">
-        <f t="shared" si="28"/>
-        <v>RW33</v>
+        <f t="shared" si="32"/>
+        <v>DE01</v>
       </c>
       <c r="G233" t="s">
         <v>443</v>
@@ -7558,7 +7551,7 @@
     </row>
     <row r="234" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="B234" t="s">
         <v>404</v>
@@ -7567,15 +7560,15 @@
         <v>274</v>
       </c>
       <c r="D234" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="E234" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3D</v>
       </c>
       <c r="F234" t="str">
-        <f t="shared" si="28"/>
-        <v>RW36</v>
+        <f t="shared" si="32"/>
+        <v>RW21</v>
       </c>
       <c r="G234" t="s">
         <v>443</v>
@@ -7584,138 +7577,138 @@
         <v>442</v>
       </c>
     </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A240" t="s">
-        <v>474</v>
-      </c>
-      <c r="B240" t="s">
-        <v>485</v>
-      </c>
-      <c r="C240" t="s">
-        <v>261</v>
-      </c>
-      <c r="D240" t="s">
-        <v>496</v>
-      </c>
-      <c r="E240" t="str">
-        <f t="shared" ref="E240:E247" si="29">IF(ISNUMBER(SEARCH("M2D",A240)),"2D","3D")</f>
-        <v>3D</v>
-      </c>
-      <c r="F240" t="str">
-        <f t="shared" ref="F240:F247" si="30">RIGHT(A240, 4)</f>
-        <v>3D01</v>
-      </c>
-      <c r="G240" t="s">
-        <v>508</v>
-      </c>
-      <c r="H240" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A241" t="s">
-        <v>475</v>
-      </c>
-      <c r="B241" t="s">
-        <v>486</v>
-      </c>
-      <c r="C241" t="s">
-        <v>190</v>
-      </c>
-      <c r="D241" t="s">
-        <v>501</v>
-      </c>
-      <c r="E241" t="str">
-        <f t="shared" si="29"/>
-        <v>3D</v>
-      </c>
-      <c r="F241" t="str">
-        <f t="shared" si="30"/>
-        <v>3D01</v>
-      </c>
-      <c r="G241" t="s">
-        <v>508</v>
-      </c>
-      <c r="H241" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A242" t="s">
-        <v>476</v>
-      </c>
-      <c r="B242" t="s">
-        <v>487</v>
-      </c>
-      <c r="C242" t="s">
-        <v>494</v>
-      </c>
-      <c r="D242" t="s">
-        <v>506</v>
-      </c>
-      <c r="E242" t="str">
-        <f t="shared" si="29"/>
-        <v>3D</v>
-      </c>
-      <c r="F242" t="str">
-        <f t="shared" si="30"/>
-        <v>EW40</v>
-      </c>
-      <c r="G242" t="s">
-        <v>508</v>
-      </c>
-      <c r="H242" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A243" t="s">
-        <v>477</v>
-      </c>
-      <c r="B243" t="s">
-        <v>488</v>
-      </c>
-      <c r="C243" t="s">
-        <v>471</v>
-      </c>
-      <c r="D243" t="s">
-        <v>497</v>
-      </c>
-      <c r="E243" t="str">
-        <f t="shared" si="29"/>
-        <v>3D</v>
-      </c>
-      <c r="F243" t="str">
-        <f t="shared" si="30"/>
-        <v>DE01</v>
-      </c>
-      <c r="G243" t="s">
-        <v>508</v>
-      </c>
-      <c r="H243" t="s">
-        <v>507</v>
+    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>438</v>
+      </c>
+      <c r="B235" t="s">
+        <v>404</v>
+      </c>
+      <c r="C235" t="s">
+        <v>274</v>
+      </c>
+      <c r="D235" t="s">
+        <v>424</v>
+      </c>
+      <c r="E235" t="str">
+        <f t="shared" si="31"/>
+        <v>3D</v>
+      </c>
+      <c r="F235" t="str">
+        <f t="shared" si="32"/>
+        <v>RW31</v>
+      </c>
+      <c r="G235" t="s">
+        <v>443</v>
+      </c>
+      <c r="H235" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>439</v>
+      </c>
+      <c r="B236" t="s">
+        <v>404</v>
+      </c>
+      <c r="C236" t="s">
+        <v>274</v>
+      </c>
+      <c r="D236" t="s">
+        <v>425</v>
+      </c>
+      <c r="E236" t="str">
+        <f t="shared" si="31"/>
+        <v>3D</v>
+      </c>
+      <c r="F236" t="str">
+        <f t="shared" si="32"/>
+        <v>RW32</v>
+      </c>
+      <c r="G236" t="s">
+        <v>443</v>
+      </c>
+      <c r="H236" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>440</v>
+      </c>
+      <c r="B237" t="s">
+        <v>404</v>
+      </c>
+      <c r="C237" t="s">
+        <v>274</v>
+      </c>
+      <c r="D237" t="s">
+        <v>415</v>
+      </c>
+      <c r="E237" t="str">
+        <f t="shared" si="31"/>
+        <v>3D</v>
+      </c>
+      <c r="F237" t="str">
+        <f t="shared" si="32"/>
+        <v>RW33</v>
+      </c>
+      <c r="G237" t="s">
+        <v>443</v>
+      </c>
+      <c r="H237" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>441</v>
+      </c>
+      <c r="B238" t="s">
+        <v>404</v>
+      </c>
+      <c r="C238" t="s">
+        <v>274</v>
+      </c>
+      <c r="D238" t="s">
+        <v>426</v>
+      </c>
+      <c r="E238" t="str">
+        <f t="shared" si="31"/>
+        <v>3D</v>
+      </c>
+      <c r="F238" t="str">
+        <f t="shared" si="32"/>
+        <v>RW36</v>
+      </c>
+      <c r="G238" t="s">
+        <v>443</v>
+      </c>
+      <c r="H238" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="244" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="B244" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="C244" t="s">
-        <v>191</v>
+        <v>261</v>
       </c>
       <c r="D244" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E244" t="str">
-        <f t="shared" si="29"/>
-        <v>2D</v>
+        <f t="shared" ref="E244:E251" si="33">IF(ISNUMBER(SEARCH("M2D",A244)),"2D","3D")</f>
+        <v>3D</v>
       </c>
       <c r="F244" t="str">
-        <f t="shared" si="30"/>
-        <v>DE01</v>
+        <f t="shared" ref="F244:F251" si="34">RIGHT(A244, 4)</f>
+        <v>3D01</v>
       </c>
       <c r="G244" t="s">
         <v>508</v>
@@ -7726,24 +7719,24 @@
     </row>
     <row r="245" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="B245" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="C245" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D245" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="E245" t="str">
-        <f t="shared" si="29"/>
-        <v>2D</v>
+        <f t="shared" si="33"/>
+        <v>3D</v>
       </c>
       <c r="F245" t="str">
-        <f t="shared" si="30"/>
-        <v>DE01</v>
+        <f t="shared" si="34"/>
+        <v>3D01</v>
       </c>
       <c r="G245" t="s">
         <v>508</v>
@@ -7754,24 +7747,24 @@
     </row>
     <row r="246" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="B246" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="C246" t="s">
-        <v>190</v>
+        <v>494</v>
       </c>
       <c r="D246" t="s">
-        <v>500</v>
+        <v>506</v>
       </c>
       <c r="E246" t="str">
-        <f t="shared" si="29"/>
-        <v>2D</v>
+        <f t="shared" si="33"/>
+        <v>3D</v>
       </c>
       <c r="F246" t="str">
-        <f t="shared" si="30"/>
-        <v>DE01</v>
+        <f t="shared" si="34"/>
+        <v>EW40</v>
       </c>
       <c r="G246" t="s">
         <v>508</v>
@@ -7782,23 +7775,23 @@
     </row>
     <row r="247" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="B247" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="C247" t="s">
-        <v>184</v>
+        <v>471</v>
       </c>
       <c r="D247" t="s">
-        <v>233</v>
+        <v>497</v>
       </c>
       <c r="E247" t="str">
-        <f t="shared" si="29"/>
-        <v>2D</v>
+        <f t="shared" si="33"/>
+        <v>3D</v>
       </c>
       <c r="F247" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>DE01</v>
       </c>
       <c r="G247" t="s">
@@ -7810,23 +7803,23 @@
     </row>
     <row r="248" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="B248" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C248" t="s">
-        <v>495</v>
+        <v>191</v>
       </c>
       <c r="D248" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
       <c r="E248" t="str">
-        <f t="shared" ref="E248:E251" si="31">IF(ISNUMBER(SEARCH("M2D",A248)),"2D","3D")</f>
+        <f t="shared" si="33"/>
         <v>2D</v>
       </c>
       <c r="F248" t="str">
-        <f t="shared" ref="F248:F251" si="32">RIGHT(A248, 4)</f>
+        <f t="shared" si="34"/>
         <v>DE01</v>
       </c>
       <c r="G248" t="s">
@@ -7838,24 +7831,24 @@
     </row>
     <row r="249" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="B249" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="C249" t="s">
-        <v>494</v>
+        <v>189</v>
       </c>
       <c r="D249" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="E249" t="str">
-        <f t="shared" si="31"/>
-        <v>3D</v>
+        <f t="shared" si="33"/>
+        <v>2D</v>
       </c>
       <c r="F249" t="str">
-        <f t="shared" si="32"/>
-        <v>EW01</v>
+        <f t="shared" si="34"/>
+        <v>DE01</v>
       </c>
       <c r="G249" t="s">
         <v>508</v>
@@ -7866,24 +7859,24 @@
     </row>
     <row r="250" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="B250" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C250" t="s">
-        <v>494</v>
+        <v>190</v>
       </c>
       <c r="D250" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="E250" t="str">
-        <f t="shared" si="31"/>
-        <v>3D</v>
+        <f t="shared" si="33"/>
+        <v>2D</v>
       </c>
       <c r="F250" t="str">
-        <f t="shared" si="32"/>
-        <v>TR01</v>
+        <f t="shared" si="34"/>
+        <v>DE01</v>
       </c>
       <c r="G250" t="s">
         <v>508</v>
@@ -7894,29 +7887,141 @@
     </row>
     <row r="251" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="B251" t="s">
-        <v>487</v>
+        <v>493</v>
       </c>
       <c r="C251" t="s">
-        <v>494</v>
+        <v>184</v>
       </c>
       <c r="D251" t="s">
-        <v>504</v>
+        <v>233</v>
       </c>
       <c r="E251" t="str">
-        <f t="shared" si="31"/>
-        <v>3D</v>
+        <f t="shared" si="33"/>
+        <v>2D</v>
       </c>
       <c r="F251" t="str">
-        <f t="shared" si="32"/>
-        <v>TR02</v>
+        <f t="shared" si="34"/>
+        <v>DE01</v>
       </c>
       <c r="G251" t="s">
         <v>508</v>
       </c>
       <c r="H251" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>482</v>
+      </c>
+      <c r="B252" t="s">
+        <v>491</v>
+      </c>
+      <c r="C252" t="s">
+        <v>495</v>
+      </c>
+      <c r="D252" t="s">
+        <v>505</v>
+      </c>
+      <c r="E252" t="str">
+        <f t="shared" ref="E252:E255" si="35">IF(ISNUMBER(SEARCH("M2D",A252)),"2D","3D")</f>
+        <v>2D</v>
+      </c>
+      <c r="F252" t="str">
+        <f t="shared" ref="F252:F255" si="36">RIGHT(A252, 4)</f>
+        <v>DE01</v>
+      </c>
+      <c r="G252" t="s">
+        <v>508</v>
+      </c>
+      <c r="H252" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>483</v>
+      </c>
+      <c r="B253" t="s">
+        <v>487</v>
+      </c>
+      <c r="C253" t="s">
+        <v>494</v>
+      </c>
+      <c r="D253" t="s">
+        <v>502</v>
+      </c>
+      <c r="E253" t="str">
+        <f t="shared" si="35"/>
+        <v>3D</v>
+      </c>
+      <c r="F253" t="str">
+        <f t="shared" si="36"/>
+        <v>EW01</v>
+      </c>
+      <c r="G253" t="s">
+        <v>508</v>
+      </c>
+      <c r="H253" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>484</v>
+      </c>
+      <c r="B254" t="s">
+        <v>487</v>
+      </c>
+      <c r="C254" t="s">
+        <v>494</v>
+      </c>
+      <c r="D254" t="s">
+        <v>503</v>
+      </c>
+      <c r="E254" t="str">
+        <f t="shared" si="35"/>
+        <v>3D</v>
+      </c>
+      <c r="F254" t="str">
+        <f t="shared" si="36"/>
+        <v>TR01</v>
+      </c>
+      <c r="G254" t="s">
+        <v>508</v>
+      </c>
+      <c r="H254" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>492</v>
+      </c>
+      <c r="B255" t="s">
+        <v>487</v>
+      </c>
+      <c r="C255" t="s">
+        <v>494</v>
+      </c>
+      <c r="D255" t="s">
+        <v>504</v>
+      </c>
+      <c r="E255" t="str">
+        <f t="shared" si="35"/>
+        <v>3D</v>
+      </c>
+      <c r="F255" t="str">
+        <f t="shared" si="36"/>
+        <v>TR02</v>
+      </c>
+      <c r="G255" t="s">
+        <v>508</v>
+      </c>
+      <c r="H255" t="s">
         <v>507</v>
       </c>
     </row>

</xml_diff>